<commit_message>
deleted extra variables dna
</commit_message>
<xml_diff>
--- a/signif_estim_univar_glm.xlsx
+++ b/signif_estim_univar_glm.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t xml:space="preserve">term</t>
   </si>
@@ -44,235 +44,238 @@
     <t xml:space="preserve">(Intercept)</t>
   </si>
   <si>
-    <t xml:space="preserve">Ventilation ~ `Sex`</t>
+    <t xml:space="preserve">Outcome ~ `Sex`</t>
   </si>
   <si>
     <t xml:space="preserve">yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Ventilation ~ `Age`</t>
+    <t xml:space="preserve">Outcome ~ `Age`</t>
   </si>
   <si>
     <t xml:space="preserve">Age</t>
   </si>
   <si>
-    <t xml:space="preserve">Ventilation ~ `anti-HCV`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `Hbs_AG`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hbs_AGYes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `Pneumonia`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PneumoniaYes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `Infection`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InfectionYes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `diseaseGroup`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diseaseGroupHypoxia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `CGS`</t>
+    <t xml:space="preserve">Outcome ~ `anti-HCV`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`anti-HCV`2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `Hbs_AG`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `LMCA`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `Pneumonia`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `Infection`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `diseaseGroup`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diseaseGroupTBI</t>
   </si>
   <si>
     <t xml:space="preserve">CGS</t>
   </si>
   <si>
-    <t xml:space="preserve">Ventilation ~ `CCI_1d`</t>
+    <t xml:space="preserve">Outcome ~ `CGS`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `CCI_1d`</t>
   </si>
   <si>
     <t xml:space="preserve">CCI_1d</t>
   </si>
   <si>
-    <t xml:space="preserve">Ventilation ~ `CIRS-G_sum_1d`</t>
+    <t xml:space="preserve">Outcome ~ `CIRS-G_sum_1d`</t>
   </si>
   <si>
     <t xml:space="preserve">`CIRS-G_sum_1d`</t>
   </si>
   <si>
-    <t xml:space="preserve">Ventilation ~ `CIRS-G_pathology_1d`</t>
+    <t xml:space="preserve">Outcome ~ `CIRS-G_pathology_1d`</t>
   </si>
   <si>
     <t xml:space="preserve">`CIRS-G_pathology_1d`</t>
   </si>
   <si>
-    <t xml:space="preserve">Ventilation ~ `CIRS-G_severity_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">`CIRS-G_severity_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `FOUR_1d`</t>
+    <t xml:space="preserve">Outcome ~ `CIRS-G_severity_1d`</t>
   </si>
   <si>
     <t xml:space="preserve">FOUR_1d</t>
   </si>
   <si>
-    <t xml:space="preserve">Ventilation ~ `SOFA_1d`</t>
+    <t xml:space="preserve">Outcome ~ `FOUR_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `SOFA_1d`</t>
   </si>
   <si>
     <t xml:space="preserve">SOFA_1d</t>
   </si>
   <si>
-    <t xml:space="preserve">Ventilation ~ `exDNA_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `8ohdg_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `WBC_1d`</t>
+    <t xml:space="preserve">Outcome ~ `exDNA_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `8ohdg_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `WBC_1d`</t>
   </si>
   <si>
     <t xml:space="preserve">WBC_1d</t>
   </si>
   <si>
-    <t xml:space="preserve">Ventilation ~ `NEU_#_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `LYM_#_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `PLT_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `Lactate_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `Creatinine_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `ALT_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `AST_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `Albumin_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Albumin_1d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `Alcaline_phosphatase_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alcaline_phosphatase_1d</t>
+    <t xml:space="preserve">Outcome ~ `NEU_#_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`NEU_#_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `LYM_#_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `PLT_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `Lactate_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `Creatinine_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `ALT_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `AST_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `Albumin_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `Alcaline_phosphatase_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `Uric_acid_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uric_acid_1d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `Urea_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `GGT_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `Chloride_1d`</t>
   </si>
   <si>
     <t xml:space="preserve">no</t>
   </si>
   <si>
-    <t xml:space="preserve">Ventilation ~ `Urea_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Urea_1d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `GGT_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GGT_1d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `Sodium_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sodium_1d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `Chloride_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chloride_1d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `APTT_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `INR_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `Fibrinogen_1d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `PT_1d`</t>
+    <t xml:space="preserve">Outcome ~ `APTT_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `INR_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `Fibrinogen_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `PT_1d`</t>
   </si>
   <si>
     <t xml:space="preserve">PT_1d</t>
   </si>
   <si>
-    <t xml:space="preserve">Ventilation ~ `Uroseptic_infection`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `Sepsis/septic_shock`</t>
+    <t xml:space="preserve">Outcome ~ `Uroseptic_infection`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `Sepsis/septic_shock`</t>
   </si>
   <si>
     <t xml:space="preserve">`Sepsis/septic_shock`Yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Ventilation ~ `ICU_FSCCRR_d`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ICU_FSCCRR_d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `FSCCRR_bed-days`</t>
+    <t xml:space="preserve">Outcome ~ `Ventilation_demand`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventilation_demand1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `Pneuminia_deterioration_d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pneuminia_deterioration_d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `Ventilation_d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventilation_d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `ICU_FSCCRR_d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `FSCCRR_bed-days`</t>
   </si>
   <si>
     <t xml:space="preserve">`FSCCRR_bed-days`</t>
   </si>
   <si>
-    <t xml:space="preserve">Ventilation ~ `Pneumonia_at_FSCCRR`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pneumonia_at_FSCCRRYes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `8ohdg 1d log`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `BD_group`</t>
+    <t xml:space="preserve">Outcome ~ `Pneumonia_at_FSCCRR`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pneumonia_at_FSCCRR1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `8ohdg 1d log`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `BD_group`</t>
   </si>
   <si>
     <t xml:space="preserve">BD_group30-46</t>
   </si>
   <si>
+    <t xml:space="preserve">BD_group46-67</t>
+  </si>
+  <si>
     <t xml:space="preserve">BD_group67-401</t>
   </si>
   <si>
-    <t xml:space="preserve">Ventilation ~ `HTR1A_rs6295`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `OLR1_rs11053646`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `NRF2_rs6726395`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `AGTR1_rs275651`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `AQP5_rs3759129`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `TLR9_rs352162`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `TLR9_rs187084`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventilation ~ `AQP5_rs3736309`</t>
+    <t xml:space="preserve">Outcome ~ `HTR1A_rs6295`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `OLR1_rs11053646`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `NRF2_rs6726395`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `AQP5_rs3759129`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `TLR9_rs352162`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `TLR9_rs187084`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `AQP5_rs3736309`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome ~ `NLR_1d`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLR_1d</t>
   </si>
 </sst>
 </file>
@@ -638,22 +641,22 @@
         <v>9</v>
       </c>
       <c r="B2" t="n">
-        <v>0.44</v>
+        <v>0.14</v>
       </c>
       <c r="C2" t="n">
-        <v>0.16</v>
+        <v>0.21</v>
       </c>
       <c r="D2" t="n">
-        <v>-4.95</v>
+        <v>-9.04</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.32</v>
+        <v>0.09</v>
       </c>
       <c r="G2" t="n">
-        <v>0.61</v>
+        <v>0.22</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
@@ -667,22 +670,22 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>0.18</v>
+        <v>0.02</v>
       </c>
       <c r="C3" t="n">
-        <v>0.37</v>
+        <v>0.56</v>
       </c>
       <c r="D3" t="n">
-        <v>-4.61</v>
+        <v>-7.04</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.08</v>
+        <v>0.01</v>
       </c>
       <c r="G3" t="n">
-        <v>0.37</v>
+        <v>0.06</v>
       </c>
       <c r="H3" t="s">
         <v>12</v>
@@ -696,22 +699,22 @@
         <v>13</v>
       </c>
       <c r="B4" t="n">
-        <v>1.01</v>
+        <v>1.03</v>
       </c>
       <c r="C4" t="n">
         <v>0.01</v>
       </c>
       <c r="D4" t="n">
-        <v>2.03</v>
+        <v>3.94</v>
       </c>
       <c r="E4" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>1.02</v>
       </c>
       <c r="G4" t="n">
-        <v>1.03</v>
+        <v>1.05</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
@@ -725,22 +728,22 @@
         <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>0.39</v>
+        <v>0.13</v>
       </c>
       <c r="C5" t="n">
-        <v>0.12</v>
+        <v>0.16</v>
       </c>
       <c r="D5" t="n">
-        <v>-7.74</v>
+        <v>-12.78</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.31</v>
+        <v>0.09</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5</v>
+        <v>0.17</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
@@ -751,28 +754,28 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B6" t="n">
-        <v>0.38</v>
+        <v>1.89</v>
       </c>
       <c r="C6" t="n">
-        <v>0.12</v>
+        <v>0.28</v>
       </c>
       <c r="D6" t="n">
-        <v>-8.01</v>
+        <v>2.26</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="F6" t="n">
-        <v>0.29</v>
+        <v>1.07</v>
       </c>
       <c r="G6" t="n">
-        <v>0.48</v>
+        <v>3.27</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I6" t="s">
         <v>11</v>
@@ -780,28 +783,28 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-12.69</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="H7" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" t="n">
-        <v>4.44</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="D7" t="n">
-        <v>2.01</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1.07</v>
-      </c>
-      <c r="G7" t="n">
-        <v>21.99</v>
-      </c>
-      <c r="H7" t="s">
-        <v>15</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
@@ -812,22 +815,22 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>0.22</v>
+        <v>0.1</v>
       </c>
       <c r="C8" t="n">
-        <v>0.16</v>
+        <v>1.05</v>
       </c>
       <c r="D8" t="n">
-        <v>-9.44</v>
+        <v>-2.2</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="F8" t="n">
-        <v>0.16</v>
+        <v>0.01</v>
       </c>
       <c r="G8" t="n">
-        <v>0.3</v>
+        <v>0.52</v>
       </c>
       <c r="H8" t="s">
         <v>17</v>
@@ -838,28 +841,28 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-11.19</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="H9" t="s">
         <v>18</v>
-      </c>
-      <c r="B9" t="n">
-        <v>3.02</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="D9" t="n">
-        <v>5</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1.97</v>
-      </c>
-      <c r="G9" t="n">
-        <v>4.69</v>
-      </c>
-      <c r="H9" t="s">
-        <v>17</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
@@ -870,22 +873,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.17</v>
+        <v>0.13</v>
       </c>
       <c r="C10" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="D10" t="n">
-        <v>-9.1</v>
+        <v>-10.13</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.12</v>
+        <v>0.09</v>
       </c>
       <c r="G10" t="n">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="H10" t="s">
         <v>19</v>
@@ -896,28 +899,28 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-6.83</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="H11" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" t="n">
-        <v>3.54</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="D11" t="n">
-        <v>5.39</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>2.26</v>
-      </c>
-      <c r="G11" t="n">
-        <v>5.68</v>
-      </c>
-      <c r="H11" t="s">
-        <v>19</v>
       </c>
       <c r="I11" t="s">
         <v>11</v>
@@ -925,28 +928,28 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B12" t="n">
-        <v>0.32</v>
+        <v>0.37</v>
       </c>
       <c r="C12" t="n">
-        <v>0.23</v>
+        <v>0.47</v>
       </c>
       <c r="D12" t="n">
-        <v>-4.89</v>
+        <v>-2.11</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2</v>
+        <v>0.14</v>
       </c>
       <c r="G12" t="n">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="H12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
@@ -957,25 +960,25 @@
         <v>22</v>
       </c>
       <c r="B13" t="n">
-        <v>2.43</v>
+        <v>0.85</v>
       </c>
       <c r="C13" t="n">
-        <v>0.42</v>
+        <v>0.04</v>
       </c>
       <c r="D13" t="n">
-        <v>2.14</v>
+        <v>-3.98</v>
       </c>
       <c r="E13" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>1.07</v>
+        <v>0.79</v>
       </c>
       <c r="G13" t="n">
-        <v>5.5</v>
+        <v>0.92</v>
       </c>
       <c r="H13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
@@ -986,25 +989,25 @@
         <v>9</v>
       </c>
       <c r="B14" t="n">
-        <v>16.34</v>
+        <v>0.02</v>
       </c>
       <c r="C14" t="n">
-        <v>0.48</v>
+        <v>0.45</v>
       </c>
       <c r="D14" t="n">
-        <v>5.84</v>
+        <v>-8.52</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>6.51</v>
+        <v>0.01</v>
       </c>
       <c r="G14" t="n">
-        <v>42.65</v>
+        <v>0.05</v>
       </c>
       <c r="H14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I14" t="s">
         <v>11</v>
@@ -1012,28 +1015,28 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="D15" t="n">
+        <v>4.93</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="H15" t="s">
         <v>24</v>
-      </c>
-      <c r="B15" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-7.96</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.68</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="H15" t="s">
-        <v>23</v>
       </c>
       <c r="I15" t="s">
         <v>11</v>
@@ -1044,25 +1047,25 @@
         <v>9</v>
       </c>
       <c r="B16" t="n">
-        <v>0.13</v>
+        <v>0.03</v>
       </c>
       <c r="C16" t="n">
-        <v>0.31</v>
+        <v>0.42</v>
       </c>
       <c r="D16" t="n">
-        <v>-6.54</v>
+        <v>-8.38</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.07</v>
+        <v>0.01</v>
       </c>
       <c r="G16" t="n">
-        <v>0.24</v>
+        <v>0.06</v>
       </c>
       <c r="H16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I16" t="s">
         <v>11</v>
@@ -1070,16 +1073,16 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" t="n">
-        <v>1.14</v>
+        <v>1.11</v>
       </c>
       <c r="C17" t="n">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="D17" t="n">
-        <v>3.67</v>
+        <v>4.43</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -1088,10 +1091,10 @@
         <v>1.06</v>
       </c>
       <c r="G17" t="n">
-        <v>1.23</v>
+        <v>1.16</v>
       </c>
       <c r="H17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
@@ -1105,22 +1108,22 @@
         <v>0.03</v>
       </c>
       <c r="C18" t="n">
-        <v>0.38</v>
+        <v>0.42</v>
       </c>
       <c r="D18" t="n">
-        <v>-8.95</v>
+        <v>-8.05</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="G18" t="n">
-        <v>0.07</v>
+        <v>0.08</v>
       </c>
       <c r="H18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I18" t="s">
         <v>11</v>
@@ -1128,28 +1131,28 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D19" t="n">
+        <v>4</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="H19" t="s">
         <v>28</v>
-      </c>
-      <c r="B19" t="n">
-        <v>1.17</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="D19" t="n">
-        <v>6.93</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" t="n">
-        <v>1.12</v>
-      </c>
-      <c r="G19" t="n">
-        <v>1.23</v>
-      </c>
-      <c r="H19" t="s">
-        <v>27</v>
       </c>
       <c r="I19" t="s">
         <v>11</v>
@@ -1160,13 +1163,13 @@
         <v>9</v>
       </c>
       <c r="B20" t="n">
-        <v>0.07</v>
+        <v>0.13</v>
       </c>
       <c r="C20" t="n">
-        <v>0.34</v>
+        <v>0.71</v>
       </c>
       <c r="D20" t="n">
-        <v>-7.86</v>
+        <v>-2.85</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -1175,10 +1178,10 @@
         <v>0.03</v>
       </c>
       <c r="G20" t="n">
-        <v>0.13</v>
+        <v>0.53</v>
       </c>
       <c r="H20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I20" t="s">
         <v>11</v>
@@ -1186,28 +1189,28 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" t="n">
-        <v>1.32</v>
+        <v>0.83</v>
       </c>
       <c r="C21" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="D21" t="n">
-        <v>5.46</v>
+        <v>-4.79</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>1.2</v>
+        <v>0.77</v>
       </c>
       <c r="G21" t="n">
-        <v>1.47</v>
+        <v>0.9</v>
       </c>
       <c r="H21" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I21" t="s">
         <v>11</v>
@@ -1221,22 +1224,22 @@
         <v>0.08</v>
       </c>
       <c r="C22" t="n">
-        <v>0.58</v>
+        <v>0.21</v>
       </c>
       <c r="D22" t="n">
-        <v>-4.36</v>
+        <v>-11.84</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="G22" t="n">
-        <v>0.25</v>
+        <v>0.12</v>
       </c>
       <c r="H22" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I22" t="s">
         <v>11</v>
@@ -1244,28 +1247,28 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B23" t="n">
-        <v>1.82</v>
+        <v>1.24</v>
       </c>
       <c r="C23" t="n">
-        <v>0.22</v>
+        <v>0.05</v>
       </c>
       <c r="D23" t="n">
-        <v>2.7</v>
+        <v>4.16</v>
       </c>
       <c r="E23" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>1.18</v>
+        <v>1.12</v>
       </c>
       <c r="G23" t="n">
-        <v>2.82</v>
+        <v>1.38</v>
       </c>
       <c r="H23" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I23" t="s">
         <v>11</v>
@@ -1276,25 +1279,25 @@
         <v>9</v>
       </c>
       <c r="B24" t="n">
-        <v>3006.74</v>
+        <v>0.19</v>
       </c>
       <c r="C24" t="n">
-        <v>0.9</v>
+        <v>0.21</v>
       </c>
       <c r="D24" t="n">
-        <v>8.9</v>
+        <v>-7.74</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>556.83</v>
+        <v>0.12</v>
       </c>
       <c r="G24" t="n">
-        <v>19023.14</v>
+        <v>0.29</v>
       </c>
       <c r="H24" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I24" t="s">
         <v>11</v>
@@ -1302,28 +1305,28 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="B25" t="n">
-        <v>0.52</v>
+        <v>0.19</v>
       </c>
       <c r="C25" t="n">
-        <v>0.07</v>
+        <v>0.18</v>
       </c>
       <c r="D25" t="n">
-        <v>-10.06</v>
+        <v>-9.34</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>0.45</v>
+        <v>0.14</v>
       </c>
       <c r="G25" t="n">
-        <v>0.59</v>
+        <v>0.27</v>
       </c>
       <c r="H25" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I25" t="s">
         <v>11</v>
@@ -1334,25 +1337,25 @@
         <v>9</v>
       </c>
       <c r="B26" t="n">
-        <v>0.11</v>
+        <v>0.06</v>
       </c>
       <c r="C26" t="n">
-        <v>0.21</v>
+        <v>0.35</v>
       </c>
       <c r="D26" t="n">
-        <v>-10.45</v>
+        <v>-8.01</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>0.07</v>
+        <v>0.03</v>
       </c>
       <c r="G26" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
       <c r="H26" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I26" t="s">
         <v>11</v>
@@ -1360,28 +1363,28 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B27" t="n">
-        <v>1.58</v>
+        <v>1.1</v>
       </c>
       <c r="C27" t="n">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="D27" t="n">
-        <v>7.18</v>
+        <v>2.91</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>1.4</v>
+        <v>1.03</v>
       </c>
       <c r="G27" t="n">
-        <v>1.79</v>
+        <v>1.17</v>
       </c>
       <c r="H27" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I27" t="s">
         <v>11</v>
@@ -1392,25 +1395,25 @@
         <v>9</v>
       </c>
       <c r="B28" t="n">
-        <v>0.28</v>
+        <v>0.1</v>
       </c>
       <c r="C28" t="n">
-        <v>0.19</v>
+        <v>0.24</v>
       </c>
       <c r="D28" t="n">
-        <v>-6.64</v>
+        <v>-9.57</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>0.19</v>
+        <v>0.06</v>
       </c>
       <c r="G28" t="n">
-        <v>0.41</v>
+        <v>0.16</v>
       </c>
       <c r="H28" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I28" t="s">
         <v>11</v>
@@ -1418,28 +1421,28 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B29" t="n">
-        <v>0.33</v>
+        <v>1.06</v>
       </c>
       <c r="C29" t="n">
-        <v>0.17</v>
+        <v>0.03</v>
       </c>
       <c r="D29" t="n">
-        <v>-6.48</v>
+        <v>2.18</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="F29" t="n">
-        <v>0.24</v>
+        <v>1.01</v>
       </c>
       <c r="G29" t="n">
-        <v>0.46</v>
+        <v>1.13</v>
       </c>
       <c r="H29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I29" t="s">
         <v>11</v>
@@ -1453,22 +1456,22 @@
         <v>0.19</v>
       </c>
       <c r="C30" t="n">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D30" t="n">
-        <v>-5.6</v>
+        <v>-6.74</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="G30" t="n">
-        <v>0.34</v>
+        <v>0.32</v>
       </c>
       <c r="H30" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I30" t="s">
         <v>11</v>
@@ -1476,28 +1479,28 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="B31" t="n">
-        <v>1.08</v>
+        <v>0.21</v>
       </c>
       <c r="C31" t="n">
-        <v>0.03</v>
+        <v>0.33</v>
       </c>
       <c r="D31" t="n">
-        <v>2.41</v>
+        <v>-4.65</v>
       </c>
       <c r="E31" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>1.01</v>
+        <v>0.11</v>
       </c>
       <c r="G31" t="n">
-        <v>1.14</v>
+        <v>0.4</v>
       </c>
       <c r="H31" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I31" t="s">
         <v>11</v>
@@ -1508,25 +1511,25 @@
         <v>9</v>
       </c>
       <c r="B32" t="n">
-        <v>0.26</v>
+        <v>0.15</v>
       </c>
       <c r="C32" t="n">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
       <c r="D32" t="n">
-        <v>-6.44</v>
+        <v>-8.06</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>0.17</v>
+        <v>0.1</v>
       </c>
       <c r="G32" t="n">
-        <v>0.39</v>
+        <v>0.24</v>
       </c>
       <c r="H32" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I32" t="s">
         <v>11</v>
@@ -1537,25 +1540,25 @@
         <v>9</v>
       </c>
       <c r="B33" t="n">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="C33" t="n">
-        <v>0.16</v>
+        <v>0.24</v>
       </c>
       <c r="D33" t="n">
-        <v>-5.65</v>
+        <v>-9.03</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>0.29</v>
+        <v>0.07</v>
       </c>
       <c r="G33" t="n">
-        <v>0.57</v>
+        <v>0.19</v>
       </c>
       <c r="H33" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I33" t="s">
         <v>11</v>
@@ -1566,25 +1569,25 @@
         <v>9</v>
       </c>
       <c r="B34" t="n">
-        <v>0.44</v>
+        <v>0.2</v>
       </c>
       <c r="C34" t="n">
-        <v>0.28</v>
+        <v>0.2</v>
       </c>
       <c r="D34" t="n">
-        <v>-2.92</v>
+        <v>-8.07</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>0.25</v>
+        <v>0.13</v>
       </c>
       <c r="G34" t="n">
-        <v>0.76</v>
+        <v>0.29</v>
       </c>
       <c r="H34" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I34" t="s">
         <v>11</v>
@@ -1595,25 +1598,25 @@
         <v>9</v>
       </c>
       <c r="B35" t="n">
-        <v>0.51</v>
+        <v>0.13</v>
       </c>
       <c r="C35" t="n">
-        <v>0.22</v>
+        <v>0.16</v>
       </c>
       <c r="D35" t="n">
-        <v>-3.12</v>
+        <v>-12.35</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>0.33</v>
+        <v>0.09</v>
       </c>
       <c r="G35" t="n">
-        <v>0.8</v>
+        <v>0.18</v>
       </c>
       <c r="H35" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I35" t="s">
         <v>11</v>
@@ -1624,25 +1627,25 @@
         <v>9</v>
       </c>
       <c r="B36" t="n">
-        <v>0.31</v>
+        <v>0.24</v>
       </c>
       <c r="C36" t="n">
-        <v>0.21</v>
+        <v>0.58</v>
       </c>
       <c r="D36" t="n">
-        <v>-5.58</v>
+        <v>-2.47</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="F36" t="n">
-        <v>0.21</v>
+        <v>0.1</v>
       </c>
       <c r="G36" t="n">
-        <v>0.48</v>
+        <v>0.82</v>
       </c>
       <c r="H36" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I36" t="s">
         <v>11</v>
@@ -1653,25 +1656,25 @@
         <v>9</v>
       </c>
       <c r="B37" t="n">
-        <v>0.34</v>
+        <v>0.12</v>
       </c>
       <c r="C37" t="n">
-        <v>0.14</v>
+        <v>0.29</v>
       </c>
       <c r="D37" t="n">
-        <v>-7.74</v>
+        <v>-7.22</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>0.26</v>
+        <v>0.07</v>
       </c>
       <c r="G37" t="n">
-        <v>0.45</v>
+        <v>0.22</v>
       </c>
       <c r="H37" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I37" t="s">
         <v>11</v>
@@ -1682,25 +1685,25 @@
         <v>9</v>
       </c>
       <c r="B38" t="n">
-        <v>0.35</v>
+        <v>0.05</v>
       </c>
       <c r="C38" t="n">
-        <v>0.14</v>
+        <v>0.51</v>
       </c>
       <c r="D38" t="n">
-        <v>-7.56</v>
+        <v>-6.01</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>0.26</v>
+        <v>0.02</v>
       </c>
       <c r="G38" t="n">
-        <v>0.46</v>
+        <v>0.12</v>
       </c>
       <c r="H38" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I38" t="s">
         <v>11</v>
@@ -1708,28 +1711,28 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="B39" t="n">
-        <v>26.46</v>
+        <v>1</v>
       </c>
       <c r="C39" t="n">
-        <v>0.66</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>4.99</v>
+        <v>2.2</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="F39" t="n">
-        <v>7.51</v>
+        <v>1</v>
       </c>
       <c r="G39" t="n">
-        <v>98.9</v>
+        <v>1.01</v>
       </c>
       <c r="H39" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I39" t="s">
         <v>11</v>
@@ -1737,28 +1740,28 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="B40" t="n">
-        <v>0.88</v>
+        <v>0.14</v>
       </c>
       <c r="C40" t="n">
-        <v>0.02</v>
+        <v>0.14</v>
       </c>
       <c r="D40" t="n">
-        <v>-6.42</v>
+        <v>-14.03</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>0.84</v>
+        <v>0.1</v>
       </c>
       <c r="G40" t="n">
-        <v>0.91</v>
+        <v>0.18</v>
       </c>
       <c r="H40" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="I40" t="s">
         <v>11</v>
@@ -1769,25 +1772,25 @@
         <v>9</v>
       </c>
       <c r="B41" t="n">
-        <v>0.22</v>
+        <v>0.13</v>
       </c>
       <c r="C41" t="n">
-        <v>0.25</v>
+        <v>0.28</v>
       </c>
       <c r="D41" t="n">
-        <v>-6.06</v>
+        <v>-7.11</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>0.13</v>
+        <v>0.08</v>
       </c>
       <c r="G41" t="n">
-        <v>0.35</v>
+        <v>0.23</v>
       </c>
       <c r="H41" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I41" t="s">
         <v>11</v>
@@ -1795,31 +1798,31 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="B42" t="n">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>2.01</v>
       </c>
       <c r="D42" t="n">
-        <v>1.94</v>
+        <v>-1.93</v>
       </c>
       <c r="E42" t="n">
         <v>0.05</v>
       </c>
       <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
         <v>1</v>
       </c>
-      <c r="G42" t="n">
-        <v>1.01</v>
-      </c>
       <c r="H42" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I42" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43">
@@ -1827,25 +1830,25 @@
         <v>9</v>
       </c>
       <c r="B43" t="n">
-        <v>0.21</v>
+        <v>0.16</v>
       </c>
       <c r="C43" t="n">
-        <v>0.19</v>
+        <v>0.36</v>
       </c>
       <c r="D43" t="n">
-        <v>-8.27</v>
+        <v>-5.05</v>
       </c>
       <c r="E43" t="n">
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>0.15</v>
+        <v>0.09</v>
       </c>
       <c r="G43" t="n">
-        <v>0.3</v>
+        <v>0.38</v>
       </c>
       <c r="H43" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I43" t="s">
         <v>11</v>
@@ -1853,28 +1856,28 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="B44" t="n">
-        <v>1.09</v>
+        <v>0.16</v>
       </c>
       <c r="C44" t="n">
-        <v>0.02</v>
+        <v>0.15</v>
       </c>
       <c r="D44" t="n">
-        <v>3.54</v>
+        <v>-12.59</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>1.04</v>
+        <v>0.12</v>
       </c>
       <c r="G44" t="n">
-        <v>1.14</v>
+        <v>0.22</v>
       </c>
       <c r="H44" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I44" t="s">
         <v>11</v>
@@ -1885,25 +1888,25 @@
         <v>9</v>
       </c>
       <c r="B45" t="n">
-        <v>0.17</v>
+        <v>0.11</v>
       </c>
       <c r="C45" t="n">
-        <v>0.26</v>
+        <v>0.39</v>
       </c>
       <c r="D45" t="n">
-        <v>-6.78</v>
+        <v>-5.72</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G45" t="n">
-        <v>0.28</v>
+        <v>0.22</v>
       </c>
       <c r="H45" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I45" t="s">
         <v>11</v>
@@ -1911,28 +1914,28 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>0.08</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="D46" t="n">
-        <v>2.13</v>
+        <v>-7.91</v>
       </c>
       <c r="E46" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="G46" t="n">
-        <v>1.01</v>
+        <v>0.14</v>
       </c>
       <c r="H46" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I46" t="s">
         <v>11</v>
@@ -1940,28 +1943,28 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B47" t="n">
-        <v>0</v>
+        <v>1.05</v>
       </c>
       <c r="C47" t="n">
-        <v>2.55</v>
+        <v>0.02</v>
       </c>
       <c r="D47" t="n">
-        <v>-3.74</v>
+        <v>2.34</v>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="F47" t="n">
-        <v>0</v>
+        <v>1.01</v>
       </c>
       <c r="G47" t="n">
-        <v>0.01</v>
+        <v>1.09</v>
       </c>
       <c r="H47" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I47" t="s">
         <v>11</v>
@@ -1969,28 +1972,28 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="B48" t="n">
-        <v>1.06</v>
+        <v>0.14</v>
       </c>
       <c r="C48" t="n">
-        <v>0.02</v>
+        <v>0.18</v>
       </c>
       <c r="D48" t="n">
-        <v>3.36</v>
+        <v>-10.66</v>
       </c>
       <c r="E48" t="n">
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>1.03</v>
+        <v>0.1</v>
       </c>
       <c r="G48" t="n">
-        <v>1.1</v>
+        <v>0.2</v>
       </c>
       <c r="H48" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I48" t="s">
         <v>11</v>
@@ -2001,25 +2004,25 @@
         <v>9</v>
       </c>
       <c r="B49" t="n">
-        <v>0.01</v>
+        <v>0.08</v>
       </c>
       <c r="C49" t="n">
-        <v>1.8</v>
+        <v>0.19</v>
       </c>
       <c r="D49" t="n">
-        <v>-2.65</v>
+        <v>-13.63</v>
       </c>
       <c r="E49" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="G49" t="n">
-        <v>0.26</v>
+        <v>0.11</v>
       </c>
       <c r="H49" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I49" t="s">
         <v>11</v>
@@ -2027,28 +2030,28 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B50" t="n">
-        <v>1.04</v>
+        <v>9.58</v>
       </c>
       <c r="C50" t="n">
-        <v>0.02</v>
+        <v>0.29</v>
       </c>
       <c r="D50" t="n">
-        <v>2.13</v>
+        <v>7.87</v>
       </c>
       <c r="E50" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>1</v>
+        <v>5.48</v>
       </c>
       <c r="G50" t="n">
-        <v>1.08</v>
+        <v>16.94</v>
       </c>
       <c r="H50" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I50" t="s">
         <v>11</v>
@@ -2059,25 +2062,25 @@
         <v>9</v>
       </c>
       <c r="B51" t="n">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="C51" t="n">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="D51" t="n">
-        <v>-4.72</v>
+        <v>-10.37</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="G51" t="n">
-        <v>0.36</v>
+        <v>0.05</v>
       </c>
       <c r="H51" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I51" t="s">
         <v>11</v>
@@ -2085,28 +2088,28 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="B52" t="n">
-        <v>0.35</v>
+        <v>20.1</v>
       </c>
       <c r="C52" t="n">
-        <v>0.12</v>
+        <v>0.39</v>
       </c>
       <c r="D52" t="n">
-        <v>-9.04</v>
+        <v>7.66</v>
       </c>
       <c r="E52" t="n">
         <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>0.27</v>
+        <v>9.86</v>
       </c>
       <c r="G52" t="n">
-        <v>0.43</v>
+        <v>46.67</v>
       </c>
       <c r="H52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I52" t="s">
         <v>11</v>
@@ -2117,25 +2120,25 @@
         <v>9</v>
       </c>
       <c r="B53" t="n">
-        <v>0.21</v>
+        <v>0.05</v>
       </c>
       <c r="C53" t="n">
-        <v>0.33</v>
+        <v>0.48</v>
       </c>
       <c r="D53" t="n">
-        <v>-4.75</v>
+        <v>-6.06</v>
       </c>
       <c r="E53" t="n">
         <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>0.11</v>
+        <v>0.02</v>
       </c>
       <c r="G53" t="n">
-        <v>0.39</v>
+        <v>0.13</v>
       </c>
       <c r="H53" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I53" t="s">
         <v>11</v>
@@ -2143,28 +2146,28 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="B54" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="C54" t="n">
         <v>0.03</v>
       </c>
-      <c r="C54" t="n">
-        <v>0.59</v>
-      </c>
       <c r="D54" t="n">
-        <v>-6.28</v>
+        <v>3.3</v>
       </c>
       <c r="E54" t="n">
         <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>0.01</v>
+        <v>1.04</v>
       </c>
       <c r="G54" t="n">
-        <v>0.08</v>
+        <v>1.15</v>
       </c>
       <c r="H54" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I54" t="s">
         <v>11</v>
@@ -2172,28 +2175,28 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B55" t="n">
-        <v>1.21</v>
+        <v>0.12</v>
       </c>
       <c r="C55" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="D55" t="n">
-        <v>4.65</v>
+        <v>-13.84</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>1.12</v>
+        <v>0.09</v>
       </c>
       <c r="G55" t="n">
-        <v>1.32</v>
+        <v>0.16</v>
       </c>
       <c r="H55" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I55" t="s">
         <v>11</v>
@@ -2201,28 +2204,28 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="B56" t="n">
-        <v>0.31</v>
+        <v>1.01</v>
       </c>
       <c r="C56" t="n">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>-7.69</v>
+        <v>3.34</v>
       </c>
       <c r="E56" t="n">
         <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>0.23</v>
+        <v>1.01</v>
       </c>
       <c r="G56" t="n">
-        <v>0.42</v>
+        <v>1.02</v>
       </c>
       <c r="H56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I56" t="s">
         <v>11</v>
@@ -2233,25 +2236,25 @@
         <v>9</v>
       </c>
       <c r="B57" t="n">
-        <v>0.27</v>
+        <v>0.16</v>
       </c>
       <c r="C57" t="n">
-        <v>0.12</v>
+        <v>0.18</v>
       </c>
       <c r="D57" t="n">
-        <v>-10.72</v>
+        <v>-10.12</v>
       </c>
       <c r="E57" t="n">
         <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>0.21</v>
+        <v>0.11</v>
       </c>
       <c r="G57" t="n">
-        <v>0.34</v>
+        <v>0.23</v>
       </c>
       <c r="H57" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I57" t="s">
         <v>11</v>
@@ -2259,28 +2262,28 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>9</v>
       </c>
       <c r="B58" t="n">
-        <v>9.93</v>
+        <v>0.4</v>
       </c>
       <c r="C58" t="n">
-        <v>0.34</v>
+        <v>0.26</v>
       </c>
       <c r="D58" t="n">
-        <v>6.81</v>
+        <v>-3.55</v>
       </c>
       <c r="E58" t="n">
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>5.24</v>
+        <v>0.24</v>
       </c>
       <c r="G58" t="n">
-        <v>19.83</v>
+        <v>0.66</v>
       </c>
       <c r="H58" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I58" t="s">
         <v>11</v>
@@ -2288,28 +2291,28 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="B59" t="n">
-        <v>0.14</v>
+        <v>0.98</v>
       </c>
       <c r="C59" t="n">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
       <c r="D59" t="n">
-        <v>-10.79</v>
+        <v>-3.79</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>0.1</v>
+        <v>0.97</v>
       </c>
       <c r="G59" t="n">
-        <v>0.2</v>
+        <v>0.99</v>
       </c>
       <c r="H59" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I59" t="s">
         <v>11</v>
@@ -2317,28 +2320,28 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B60" t="n">
-        <v>1.02</v>
+        <v>0.12</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="D60" t="n">
-        <v>6.88</v>
+        <v>-13.02</v>
       </c>
       <c r="E60" t="n">
         <v>0</v>
       </c>
       <c r="F60" t="n">
-        <v>1.02</v>
+        <v>0.09</v>
       </c>
       <c r="G60" t="n">
-        <v>1.03</v>
+        <v>0.16</v>
       </c>
       <c r="H60" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I60" t="s">
         <v>11</v>
@@ -2346,28 +2349,28 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="B61" t="n">
-        <v>0.18</v>
+        <v>2.14</v>
       </c>
       <c r="C61" t="n">
-        <v>0.2</v>
+        <v>0.28</v>
       </c>
       <c r="D61" t="n">
-        <v>-8.62</v>
+        <v>2.71</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="F61" t="n">
-        <v>0.12</v>
+        <v>1.22</v>
       </c>
       <c r="G61" t="n">
-        <v>0.27</v>
+        <v>3.69</v>
       </c>
       <c r="H61" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I61" t="s">
         <v>11</v>
@@ -2375,28 +2378,28 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="B62" t="n">
-        <v>1.01</v>
+        <v>0.16</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>0.39</v>
       </c>
       <c r="D62" t="n">
-        <v>4.32</v>
+        <v>-4.73</v>
       </c>
       <c r="E62" t="n">
         <v>0</v>
       </c>
       <c r="F62" t="n">
-        <v>1.01</v>
+        <v>0.07</v>
       </c>
       <c r="G62" t="n">
-        <v>1.02</v>
+        <v>0.3</v>
       </c>
       <c r="H62" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I62" t="s">
         <v>11</v>
@@ -2407,25 +2410,25 @@
         <v>9</v>
       </c>
       <c r="B63" t="n">
-        <v>0.31</v>
+        <v>0.35</v>
       </c>
       <c r="C63" t="n">
-        <v>0.13</v>
+        <v>0.2</v>
       </c>
       <c r="D63" t="n">
-        <v>-9.24</v>
+        <v>-5.23</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="G63" t="n">
-        <v>0.4</v>
+        <v>0.51</v>
       </c>
       <c r="H63" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I63" t="s">
         <v>11</v>
@@ -2433,28 +2436,28 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B64" t="n">
-        <v>1.97</v>
+        <v>0.34</v>
       </c>
       <c r="C64" t="n">
-        <v>0.25</v>
+        <v>0.36</v>
       </c>
       <c r="D64" t="n">
-        <v>2.76</v>
+        <v>-3</v>
       </c>
       <c r="E64" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>1.21</v>
+        <v>0.17</v>
       </c>
       <c r="G64" t="n">
-        <v>3.19</v>
+        <v>0.68</v>
       </c>
       <c r="H64" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I64" t="s">
         <v>11</v>
@@ -2462,25 +2465,25 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="B65" t="n">
-        <v>0.47</v>
+        <v>0.2</v>
       </c>
       <c r="C65" t="n">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="D65" t="n">
-        <v>-2.54</v>
+        <v>-4</v>
       </c>
       <c r="E65" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>0.27</v>
+        <v>0.09</v>
       </c>
       <c r="G65" t="n">
-        <v>0.89</v>
+        <v>0.43</v>
       </c>
       <c r="H65" t="s">
         <v>75</v>
@@ -2491,28 +2494,28 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="B66" t="n">
-        <v>0.3</v>
+        <v>0.28</v>
       </c>
       <c r="C66" t="n">
-        <v>0.24</v>
+        <v>0.38</v>
       </c>
       <c r="D66" t="n">
-        <v>-4.93</v>
+        <v>-3.37</v>
       </c>
       <c r="E66" t="n">
         <v>0</v>
       </c>
       <c r="F66" t="n">
-        <v>0.18</v>
+        <v>0.13</v>
       </c>
       <c r="G66" t="n">
-        <v>0.48</v>
+        <v>0.57</v>
       </c>
       <c r="H66" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I66" t="s">
         <v>11</v>
@@ -2520,28 +2523,28 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="B67" t="n">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="C67" t="n">
-        <v>0.42</v>
+        <v>0.32</v>
       </c>
       <c r="D67" t="n">
-        <v>-2.85</v>
+        <v>-6.77</v>
       </c>
       <c r="E67" t="n">
         <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
       <c r="G67" t="n">
-        <v>0.67</v>
+        <v>0.21</v>
       </c>
       <c r="H67" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I67" t="s">
         <v>11</v>
@@ -2549,28 +2552,28 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="B68" t="n">
-        <v>3.32</v>
+        <v>0.15</v>
       </c>
       <c r="C68" t="n">
-        <v>0.31</v>
+        <v>0.15</v>
       </c>
       <c r="D68" t="n">
-        <v>3.89</v>
+        <v>-12.79</v>
       </c>
       <c r="E68" t="n">
         <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>1.83</v>
+        <v>0.11</v>
       </c>
       <c r="G68" t="n">
-        <v>6.16</v>
+        <v>0.2</v>
       </c>
       <c r="H68" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="I68" t="s">
         <v>11</v>
@@ -2581,25 +2584,25 @@
         <v>9</v>
       </c>
       <c r="B69" t="n">
-        <v>0.29</v>
+        <v>0.17</v>
       </c>
       <c r="C69" t="n">
-        <v>0.25</v>
+        <v>0.31</v>
       </c>
       <c r="D69" t="n">
-        <v>-5.03</v>
+        <v>-5.7</v>
       </c>
       <c r="E69" t="n">
         <v>0</v>
       </c>
       <c r="F69" t="n">
-        <v>0.17</v>
+        <v>0.09</v>
       </c>
       <c r="G69" t="n">
-        <v>0.46</v>
+        <v>0.3</v>
       </c>
       <c r="H69" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I69" t="s">
         <v>11</v>
@@ -2610,25 +2613,25 @@
         <v>9</v>
       </c>
       <c r="B70" t="n">
-        <v>0.37</v>
+        <v>0.15</v>
       </c>
       <c r="C70" t="n">
-        <v>0.12</v>
+        <v>0.19</v>
       </c>
       <c r="D70" t="n">
-        <v>-8.25</v>
+        <v>-9.97</v>
       </c>
       <c r="E70" t="n">
         <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>0.29</v>
+        <v>0.11</v>
       </c>
       <c r="G70" t="n">
-        <v>0.46</v>
+        <v>0.22</v>
       </c>
       <c r="H70" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I70" t="s">
         <v>11</v>
@@ -2639,25 +2642,25 @@
         <v>9</v>
       </c>
       <c r="B71" t="n">
-        <v>0.42</v>
+        <v>0.17</v>
       </c>
       <c r="C71" t="n">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
       <c r="D71" t="n">
-        <v>-3.34</v>
+        <v>-6.96</v>
       </c>
       <c r="E71" t="n">
         <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="G71" t="n">
-        <v>0.69</v>
+        <v>0.27</v>
       </c>
       <c r="H71" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I71" t="s">
         <v>11</v>
@@ -2668,28 +2671,28 @@
         <v>9</v>
       </c>
       <c r="B72" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="C72" t="n">
-        <v>0.78</v>
+        <v>0.3</v>
       </c>
       <c r="D72" t="n">
-        <v>-1.92</v>
+        <v>-5.18</v>
       </c>
       <c r="E72" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>0.03</v>
+        <v>0.11</v>
       </c>
       <c r="G72" t="n">
-        <v>0.86</v>
+        <v>0.36</v>
       </c>
       <c r="H72" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I72" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73">
@@ -2697,25 +2700,25 @@
         <v>9</v>
       </c>
       <c r="B73" t="n">
-        <v>0.35</v>
+        <v>0.17</v>
       </c>
       <c r="C73" t="n">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
       <c r="D73" t="n">
-        <v>-6.69</v>
+        <v>-9.53</v>
       </c>
       <c r="E73" t="n">
         <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>0.26</v>
+        <v>0.11</v>
       </c>
       <c r="G73" t="n">
-        <v>0.47</v>
+        <v>0.24</v>
       </c>
       <c r="H73" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I73" t="s">
         <v>11</v>
@@ -2726,25 +2729,25 @@
         <v>9</v>
       </c>
       <c r="B74" t="n">
-        <v>0.31</v>
+        <v>0.1</v>
       </c>
       <c r="C74" t="n">
-        <v>0.23</v>
+        <v>0.19</v>
       </c>
       <c r="D74" t="n">
-        <v>-5.08</v>
+        <v>-12.49</v>
       </c>
       <c r="E74" t="n">
         <v>0</v>
       </c>
       <c r="F74" t="n">
-        <v>0.2</v>
+        <v>0.07</v>
       </c>
       <c r="G74" t="n">
-        <v>0.48</v>
+        <v>0.14</v>
       </c>
       <c r="H74" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I74" t="s">
         <v>11</v>
@@ -2752,59 +2755,30 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="B75" t="n">
-        <v>0.27</v>
+        <v>1.07</v>
       </c>
       <c r="C75" t="n">
-        <v>0.31</v>
+        <v>0.02</v>
       </c>
       <c r="D75" t="n">
-        <v>-4.25</v>
+        <v>3.86</v>
       </c>
       <c r="E75" t="n">
         <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>0.14</v>
+        <v>1.03</v>
       </c>
       <c r="G75" t="n">
-        <v>0.47</v>
+        <v>1.1</v>
       </c>
       <c r="H75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I75" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="s">
-        <v>9</v>
-      </c>
-      <c r="B76" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="C76" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="D76" t="n">
-        <v>-6.22</v>
-      </c>
-      <c r="E76" t="n">
-        <v>0</v>
-      </c>
-      <c r="F76" t="n">
-        <v>0.27</v>
-      </c>
-      <c r="G76" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="H76" t="s">
-        <v>86</v>
-      </c>
-      <c r="I76" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>